<commit_message>
42th commit: upload activity page implmented fully
</commit_message>
<xml_diff>
--- a/OnlineBudgetAnalysisApp/UI/uploads/ProductInfo.xlsx
+++ b/OnlineBudgetAnalysisApp/UI/uploads/ProductInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINHAZ\Desktop\partially final\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINHAZ\Desktop\Upload\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
52th commit: empty space problem in project and product list page have been fixed
</commit_message>
<xml_diff>
--- a/OnlineBudgetAnalysisApp/UI/uploads/ProductInfo.xlsx
+++ b/OnlineBudgetAnalysisApp/UI/uploads/ProductInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINHAZ\Desktop\Upload\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINHAZ\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>SKU</t>
   </si>
@@ -44,30 +44,6 @@
     <t>SKU101</t>
   </si>
   <si>
-    <t>SKU102</t>
-  </si>
-  <si>
-    <t>SKU103</t>
-  </si>
-  <si>
-    <t>SKU104</t>
-  </si>
-  <si>
-    <t>SKU105</t>
-  </si>
-  <si>
-    <t>SKU106</t>
-  </si>
-  <si>
-    <t>SKU107</t>
-  </si>
-  <si>
-    <t>SKU108</t>
-  </si>
-  <si>
-    <t>SKU109</t>
-  </si>
-  <si>
     <t>VAT(%)</t>
   </si>
   <si>
@@ -80,52 +56,7 @@
     <t>Food Container</t>
   </si>
   <si>
-    <t>Water Boottle</t>
-  </si>
-  <si>
-    <t>TableWare</t>
-  </si>
-  <si>
-    <t>KitchenWare</t>
-  </si>
-  <si>
-    <t>Hanger</t>
-  </si>
-  <si>
-    <t>Cleaning</t>
-  </si>
-  <si>
-    <t>Storage</t>
-  </si>
-  <si>
-    <t>Furniture</t>
-  </si>
-  <si>
-    <t>Kids</t>
-  </si>
-  <si>
     <t>Smile Container</t>
-  </si>
-  <si>
-    <t>PolyProphelene</t>
-  </si>
-  <si>
-    <t>Vigoset</t>
-  </si>
-  <si>
-    <t>DishRack</t>
-  </si>
-  <si>
-    <t>Flip &amp; Clean</t>
-  </si>
-  <si>
-    <t>Rack</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>Tiffin Box</t>
   </si>
 </sst>
 </file>
@@ -443,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,10 +387,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -474,7 +405,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -482,10 +413,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>25</v>
@@ -505,210 +436,28 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="F3">
         <v>1.5</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4">
-        <v>40</v>
-      </c>
-      <c r="E4">
-        <v>2.5</v>
-      </c>
-      <c r="F4">
-        <v>1.5</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5">
-        <v>34</v>
-      </c>
-      <c r="E5">
-        <v>23</v>
-      </c>
-      <c r="F5">
-        <v>44</v>
-      </c>
-      <c r="G5">
         <v>5</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6">
-        <v>0.25</v>
-      </c>
-      <c r="F6">
-        <v>0.15</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7">
-        <v>60</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-      <c r="H7">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8">
-        <v>250</v>
-      </c>
-      <c r="E8">
-        <v>25</v>
-      </c>
-      <c r="F8">
-        <v>35</v>
-      </c>
-      <c r="G8">
-        <v>20</v>
-      </c>
-      <c r="H8">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9">
-        <v>175</v>
-      </c>
-      <c r="E9">
-        <v>30</v>
-      </c>
-      <c r="F9">
-        <v>18.75</v>
-      </c>
-      <c r="G9">
-        <v>15</v>
-      </c>
-      <c r="H9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10">
-        <v>35</v>
-      </c>
-      <c r="E10">
-        <v>1.5</v>
-      </c>
-      <c r="F10">
-        <v>0.15</v>
-      </c>
-      <c r="G10">
-        <v>0.53</v>
-      </c>
-      <c r="H10">
-        <v>0.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>